<commit_message>
added a docx reader program and program to create excel docs
</commit_message>
<xml_diff>
--- a/10_word_excel/favorites.xlsx
+++ b/10_word_excel/favorites.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Favorite Things" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,21 +424,55 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Pizza</t>
+          <t>Favorite Foods</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Favorite Colors</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Chocolate Cake</t>
+          <t>Pizza</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Blue</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>Chocolate Cake</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Purple</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
           <t>Broccoli</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Green</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Orange</t>
         </is>
       </c>
     </row>

</xml_diff>